<commit_message>
fixed the broken data
</commit_message>
<xml_diff>
--- a/labeled_dataset_final.xlsx
+++ b/labeled_dataset_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Kuliah\S2 ITS\Semester 2\TESIS - PROPOSAL\DATASET PREPARATION\drone-timeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Kuliah\S2 ITS\Semester 2\TESIS - PROPOSAL\DATASET PREPARATION\droner-dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D4E984-4A24-42E4-AFDE-985801382AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1EA7A0-1D38-4B5F-A3B4-43B8D961E93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="14265" windowHeight="6000" xr2:uid="{82D0CE64-A960-4197-8241-0BF67CEC3427}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{82D0CE64-A960-4197-8241-0BF67CEC3427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>